<commit_message>
2nd Commit with Recipes and delete Morbidity
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/postmorbidity.xlsx
+++ b/src/test/resources/Exceldata/postmorbidity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svatt\git\DieticianAPI-Hackathon\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE86391F-0CCC-4444-8591-429DDB0BA8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D9D855-C8D7-4AB5-B77A-CC6C7462B532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7308" yWindow="204" windowWidth="13884" windowHeight="12216" xr2:uid="{B0A98FBE-6F60-457E-ABA3-969033FE0153}"/>
+    <workbookView xWindow="864" yWindow="672" windowWidth="13884" windowHeight="12216" xr2:uid="{B0A98FBE-6F60-457E-ABA3-969033FE0153}"/>
   </bookViews>
   <sheets>
     <sheet name="PostMorbidity" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>MorbidityName</t>
   </si>
@@ -89,52 +89,19 @@
     <t xml:space="preserve">4VA6C1spondylosis      </t>
   </si>
   <si>
-    <t>12V_12V</t>
-  </si>
-  <si>
-    <t>22V_22V</t>
-  </si>
-  <si>
-    <t>32V_32V</t>
-  </si>
-  <si>
-    <t>42V_42V</t>
-  </si>
-  <si>
-    <t>52V_52V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22VB1AS1BloodTest    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">32VB2AS1BloodTest    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">42VB3AS1BloodTest    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">52VB4AS1BloodTest    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">62VB5AS1BloodTest    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">22VA1C1spondylosis       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">32VA2C1spondylosis       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">42VA3C1spondylosis       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">52VA4C1spondylosis      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">62VA5C1spondylosis      </t>
-  </si>
-  <si>
-    <t>62V_62V</t>
+    <t xml:space="preserve">10VB1AS1BloodTest    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10VB2AS1BloodTest    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10VA1C1spondylosis       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10VA2C1spondylosis       </t>
+  </si>
+  <si>
+    <t>10V_10V</t>
   </si>
 </sst>
 </file>
@@ -493,21 +460,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6196CE6F-435D-4F77-8460-EFB5280CE745}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.88671875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="17.33203125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="18.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -521,90 +488,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
+      <c r="E3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>